<commit_message>
Updated ISRG.xlsx. Added ISRG-CodeBook.md.
</commit_message>
<xml_diff>
--- a/ISRG.xlsx
+++ b/ISRG.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>fiscal year ended</t>
   </si>
@@ -27,12 +27,6 @@
   </si>
   <si>
     <t>capital expenditure</t>
-  </si>
-  <si>
-    <t>current debt</t>
-  </si>
-  <si>
-    <t>long-term debt</t>
   </si>
   <si>
     <t>recurring revenue</t>
@@ -57,12 +51,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
@@ -82,14 +77,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -320,7 +321,7 @@
     <col customWidth="1" min="3" max="3" width="10.57"/>
     <col customWidth="1" min="4" max="4" width="17.14"/>
     <col customWidth="1" min="5" max="5" width="16.71"/>
-    <col customWidth="1" min="8" max="8" width="15.71"/>
+    <col customWidth="1" min="6" max="6" width="15.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -333,149 +334,113 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2">
+      <c r="A2" s="3">
         <v>43830.0</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="4">
         <v>4478.5</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="5">
         <v>3110.2</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <v>1598.2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <v>425.6</v>
       </c>
-      <c r="F2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="F2" s="4">
         <v>3239.3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2">
+      <c r="A3" s="3">
         <v>43465.0</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>3724.2</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="5">
         <v>2604.1</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <v>1169.6</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="4">
         <v>187.4</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="F3" s="4">
         <v>2648.5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2">
+      <c r="A4" s="3">
         <v>43100.0</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>3138.2</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="5">
         <v>2202.0</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <v>1143.9</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="4">
         <v>190.7</v>
       </c>
-      <c r="F4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="F4" s="4">
         <v>2235.7</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2">
+      <c r="A5" s="3">
         <v>42735.0</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>2704.4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="5">
         <v>1892.9</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <v>1087.0</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <v>53.9</v>
       </c>
-      <c r="F5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="F5" s="4">
         <v>1923.1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2">
+      <c r="A6" s="3">
         <v>42369.0</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="4">
         <v>2384.4</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="5">
         <v>1577.9</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <v>806.2</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="4">
         <v>81.0</v>
       </c>
-      <c r="F6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="F6" s="4">
         <v>1669.5</v>
       </c>
     </row>
@@ -500,178 +465,178 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3">
+        <v>43830.0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4">
+        <v>2408.2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3">
+        <v>43830.0</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="4">
+        <v>724.2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3">
+        <v>43830.0</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4">
+        <v>106.9</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3">
+        <v>43465.0</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2">
-        <v>43830.0</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C5" s="4">
+        <v>1962.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3">
+        <v>43465.0</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4">
+        <v>635.1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3">
+        <v>43465.0</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3">
-        <v>2408.2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2">
-        <v>43830.0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="3">
-        <v>724.2</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2">
-        <v>43830.0</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
-        <v>106.9</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2">
-        <v>43465.0</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C7" s="4">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3">
+        <v>43100.0</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1636.9</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3">
+        <v>43100.0</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4">
+        <v>572.9</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3">
+        <v>43100.0</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3">
-        <v>1962.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2">
-        <v>43465.0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3">
-        <v>635.1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2">
-        <v>43465.0</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3">
-        <v>51.4</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2">
-        <v>43100.0</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C10" s="4">
+        <v>25.9</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3">
+        <v>42735.0</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1395.8</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3">
+        <v>42735.0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4">
+        <v>510.7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3">
+        <v>42735.0</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3">
-        <v>1636.9</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2">
-        <v>43100.0</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="3">
-        <v>572.9</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2">
-        <v>43100.0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3">
-        <v>25.9</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2">
-        <v>42735.0</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C13" s="4">
+        <v>16.6</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3">
+        <v>42369.0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1197.7</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3">
+        <v>42369.0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="4">
+        <v>464.8</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3">
+        <v>42369.0</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="3">
-        <v>1395.8</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2">
-        <v>42735.0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3">
-        <v>510.7</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2">
-        <v>42735.0</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="3">
-        <v>16.6</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2">
-        <v>42369.0</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1197.7</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2">
-        <v>42369.0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3">
-        <v>464.8</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2">
-        <v>42369.0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="3">
+      <c r="C16" s="4">
         <v>7.0</v>
       </c>
     </row>

</xml_diff>